<commit_message>
write and read excel
</commit_message>
<xml_diff>
--- a/data/create_user.xlsx
+++ b/data/create_user.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="12585" windowHeight="3765"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14250" windowHeight="3990"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>status</t>
   </si>
@@ -35,6 +35,12 @@
   </si>
   <si>
     <t>Hanh</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>df</t>
   </si>
 </sst>
 </file>
@@ -361,7 +367,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -369,10 +375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -402,6 +408,14 @@
       </c>
       <c r="C2" s="1"/>
     </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>